<commit_message>
mise à jour du fichier de suivi
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/obvil/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/obvil/Documents/GitHub/historiographie-theatre/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4212B8C4-5F50-5940-8772-8D026FF4156F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5DEB5A-E149-2B4D-8386-3B72FECABC0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="1060" windowWidth="22100" windowHeight="16340" xr2:uid="{094DD94C-A879-2B45-8344-342236E78D8F}"/>
+    <workbookView xWindow="4200" yWindow="620" windowWidth="22100" windowHeight="16340" xr2:uid="{094DD94C-A879-2B45-8344-342236E78D8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -27,21 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
-    <t>historiographie_010</t>
-  </si>
-  <si>
-    <t>historiographie_011</t>
-  </si>
-  <si>
-    <t>historiographie_020</t>
-  </si>
-  <si>
-    <t>historiographie_021</t>
-  </si>
-  <si>
-    <t>historiographie_022</t>
-  </si>
-  <si>
     <t>filename</t>
   </si>
   <si>
@@ -130,6 +115,21 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>napoli-signorelli_storia-critica-ed-3-10-1_1813.xml</t>
+  </si>
+  <si>
+    <t>napoli-signorelli_storia-critica-ed-3-10-2_1813.xml</t>
+  </si>
+  <si>
+    <t>rasi_comici-italiani-01-01_1897.xml</t>
+  </si>
+  <si>
+    <t>rasi_comici-italiani-01-02_1897.xml</t>
+  </si>
+  <si>
+    <t>rasi_comici-italiani-02_1897.xml</t>
   </si>
 </sst>
 </file>
@@ -532,7 +532,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,18 +543,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -565,7 +565,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -576,7 +576,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -598,7 +598,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -609,7 +609,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -620,7 +620,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -631,7 +631,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -642,7 +642,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -653,7 +653,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -664,7 +664,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -675,7 +675,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -686,7 +686,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -697,7 +697,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -708,7 +708,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
@@ -730,7 +730,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
@@ -741,7 +741,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
@@ -752,7 +752,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1">
         <v>1</v>
@@ -763,7 +763,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
         <v>1</v>
@@ -774,7 +774,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
@@ -785,7 +785,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
@@ -796,7 +796,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
@@ -807,7 +807,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>1</v>
@@ -818,7 +818,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
@@ -829,7 +829,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
@@ -840,70 +840,70 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="B29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B33" s="1">
         <f>SUM(B2:B32)</f>
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C33" s="1">
         <f>SUM(C2:C32)</f>
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>